<commit_message>
Updating the raw data following co-author comments
</commit_message>
<xml_diff>
--- a/Data/Trait_data_and_sources.xlsx
+++ b/Data/Trait_data_and_sources.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="20955" windowHeight="9465"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="20955" windowHeight="9465" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="254">
   <si>
     <t>N</t>
   </si>
@@ -703,9 +703,6 @@
     <t>Categorical variable that groups species based on distribution size: very widespread, widespread, local, scarce, rare, very rare.</t>
   </si>
   <si>
-    <t>A binary variable describing a species emergence strategy: 1) Spring emergence = highly synchronised, 2) Summer emergence = temporally dispersed  emergence</t>
-  </si>
-  <si>
     <t>Species classified using the Red List criteria</t>
   </si>
   <si>
@@ -782,6 +779,12 @@
   </si>
   <si>
     <t>Merritt, R., Moore, N. W. &amp; Eversham, B. C. (1996) Atlas of the dragonflies of Britain and Ireland. HMSO Great Britain.</t>
+  </si>
+  <si>
+    <t>Brooks, S. (2013) Pers. Comm.</t>
+  </si>
+  <si>
+    <t>A variable describing a species emergence strategy: 1) Spring emergence = highly synchronised, 2) Summer emergence = temporally dispersed  emergence, 3) Type 3 Summer = Obligatorily univoltine species.</t>
   </si>
 </sst>
 </file>
@@ -1203,9 +1206,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BR44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AN2" sqref="AN2:AN44"/>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AC1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AE44" sqref="AE44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1379,7 +1382,7 @@
         <v>201</v>
       </c>
       <c r="AO1" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AP1" s="5" t="s">
         <v>160</v>
@@ -1408,10 +1411,10 @@
     </row>
     <row r="2" spans="1:69">
       <c r="A2" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>13</v>
@@ -1487,7 +1490,7 @@
         <v>1</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AB2" s="3">
         <v>5</v>
@@ -1695,7 +1698,7 @@
         <v>1</v>
       </c>
       <c r="AV3" s="3">
-        <f>SUM(AP3:AU3)</f>
+        <f t="shared" ref="AV3:AV18" si="0">SUM(AP3:AU3)</f>
         <v>2</v>
       </c>
       <c r="AW3" s="3">
@@ -1856,7 +1859,7 @@
         <v>1</v>
       </c>
       <c r="AV4" s="3">
-        <f>SUM(AP4:AU4)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="AW4" s="3">
@@ -2023,7 +2026,7 @@
         <v>1</v>
       </c>
       <c r="AV5" s="3">
-        <f>SUM(AP5:AU5)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="AW5" s="3">
@@ -2142,10 +2145,10 @@
         <v>7</v>
       </c>
       <c r="AE6" s="3" t="s">
-        <v>145</v>
+        <v>27</v>
       </c>
       <c r="AF6" s="3">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="AG6" s="3" t="s">
         <v>145</v>
@@ -2181,7 +2184,7 @@
         <v>1</v>
       </c>
       <c r="AV6" s="3">
-        <f>SUM(AP6:AU6)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AW6" s="3">
@@ -2288,7 +2291,7 @@
         <v>1</v>
       </c>
       <c r="AA7" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AB7" s="3">
         <v>5</v>
@@ -2342,7 +2345,7 @@
         <v>1</v>
       </c>
       <c r="AV7" s="3">
-        <f>SUM(AP7:AU7)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="AW7" s="3">
@@ -2506,7 +2509,7 @@
         <v>1</v>
       </c>
       <c r="AV8" s="3">
-        <f>SUM(AP8:AU8)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="AW8" s="3">
@@ -2673,7 +2676,7 @@
         <v>1</v>
       </c>
       <c r="AV9" s="3">
-        <f>SUM(AP9:AU9)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="AW9" s="3">
@@ -2837,7 +2840,7 @@
         <v>1</v>
       </c>
       <c r="AV10" s="3">
-        <f>SUM(AP10:AU10)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="AW10" s="3">
@@ -2992,7 +2995,7 @@
         <v>1</v>
       </c>
       <c r="AV11" s="3">
-        <f>SUM(AP11:AU11)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AW11" s="3">
@@ -3147,7 +3150,7 @@
         <v>1</v>
       </c>
       <c r="AV12" s="3">
-        <f>SUM(AP12:AU12)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AW12" s="3">
@@ -3302,7 +3305,7 @@
         <v>1</v>
       </c>
       <c r="AV13" s="3">
-        <f>SUM(AP13:AU13)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AW13" s="3">
@@ -3460,7 +3463,7 @@
         <v>1</v>
       </c>
       <c r="AV14" s="3">
-        <f>SUM(AP14:AU14)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AW14" s="3">
@@ -3605,7 +3608,7 @@
         <v>1</v>
       </c>
       <c r="AV15" s="3">
-        <f>SUM(AP15:AU15)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="AW15" s="3">
@@ -3763,7 +3766,7 @@
         <v>1</v>
       </c>
       <c r="AV16" s="3">
-        <f>SUM(AP16:AU16)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AW16" s="3">
@@ -3927,7 +3930,7 @@
         <v>1</v>
       </c>
       <c r="AV17" s="3">
-        <f>SUM(AP17:AU17)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="AW17" s="3">
@@ -4088,7 +4091,7 @@
         <v>1</v>
       </c>
       <c r="AV18" s="3">
-        <f>SUM(AP18:AU18)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="AW18" s="3">
@@ -4117,10 +4120,10 @@
     </row>
     <row r="19" spans="1:69">
       <c r="A19" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>46</v>
@@ -4403,12 +4406,8 @@
       <c r="AR20" s="7">
         <v>1</v>
       </c>
-      <c r="AU20" s="7">
-        <v>1</v>
-      </c>
       <c r="AV20" s="3">
-        <f>SUM(AP20:AU20)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AW20" s="3">
         <v>3</v>
@@ -4928,10 +4927,10 @@
     </row>
     <row r="24" spans="1:69">
       <c r="A24" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>46</v>
@@ -5569,10 +5568,10 @@
     </row>
     <row r="28" spans="1:69">
       <c r="A28" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>46</v>
@@ -5624,10 +5623,10 @@
         <v>1</v>
       </c>
       <c r="S28" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="T28" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="T28" s="3" t="s">
-        <v>250</v>
       </c>
       <c r="U28" s="3">
         <v>4</v>
@@ -6049,10 +6048,10 @@
     </row>
     <row r="31" spans="1:69">
       <c r="A31" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>243</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>244</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>46</v>
@@ -6330,7 +6329,7 @@
         <v>1</v>
       </c>
       <c r="AV32" s="3">
-        <f>SUM(AP32:AU32)</f>
+        <f t="shared" ref="AV32:AV44" si="1">SUM(AP32:AU32)</f>
         <v>1</v>
       </c>
       <c r="AW32" s="3">
@@ -6488,7 +6487,7 @@
         <v>1</v>
       </c>
       <c r="AV33" s="3">
-        <f>SUM(AP33:AU33)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="AW33" s="3">
@@ -6639,7 +6638,7 @@
         <v>1</v>
       </c>
       <c r="AV34" s="3">
-        <f>SUM(AP34:AU34)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="AW34" s="3">
@@ -6803,7 +6802,7 @@
         <v>1</v>
       </c>
       <c r="AV35" s="3">
-        <f>SUM(AP35:AU35)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="AW35" s="3">
@@ -6964,7 +6963,7 @@
         <v>1</v>
       </c>
       <c r="AV36" s="3">
-        <f>SUM(AP36:AU36)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="AW36" s="3">
@@ -7122,7 +7121,7 @@
         <v>1</v>
       </c>
       <c r="AV37" s="3">
-        <f>SUM(AP37:AU37)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="AW37" s="3">
@@ -7241,10 +7240,10 @@
         <v>7</v>
       </c>
       <c r="AE38" s="3" t="s">
-        <v>145</v>
+        <v>27</v>
       </c>
       <c r="AF38" s="3">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="AG38" s="3" t="s">
         <v>50</v>
@@ -7280,7 +7279,7 @@
         <v>1</v>
       </c>
       <c r="AV38" s="3">
-        <f>SUM(AP38:AU38)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="AW38" s="3">
@@ -7447,7 +7446,7 @@
         <v>1</v>
       </c>
       <c r="AV39" s="3">
-        <f>SUM(AP39:AU39)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="AW39" s="3">
@@ -7601,7 +7600,7 @@
         <v>1</v>
       </c>
       <c r="AV40" s="3">
-        <f>SUM(AP40:AU40)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="AW40" s="3">
@@ -7739,7 +7738,7 @@
         <v>1</v>
       </c>
       <c r="AV41" s="3">
-        <f>SUM(AP41:AU41)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="AW41" s="3">
@@ -7820,7 +7819,7 @@
         <v>1</v>
       </c>
       <c r="Y42" s="3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Z42" s="3">
         <v>1</v>
@@ -7874,7 +7873,7 @@
         <v>1</v>
       </c>
       <c r="AV42" s="3">
-        <f>SUM(AP42:AU42)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AW42" s="3">
@@ -8021,7 +8020,7 @@
         <v>1</v>
       </c>
       <c r="AV43" s="3">
-        <f>SUM(AP43:AU43)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="AW43" s="3">
@@ -8102,7 +8101,7 @@
         <v>1</v>
       </c>
       <c r="Y44" s="3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Z44" s="3">
         <v>1</v>
@@ -8168,7 +8167,7 @@
         <v>1</v>
       </c>
       <c r="AV44" s="3">
-        <f>SUM(AP44:AU44)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="AW44" s="3">
@@ -8210,10 +8209,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8322,6 +8321,14 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>252</v>
       </c>
     </row>
@@ -8334,14 +8341,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="146.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="183.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -8373,7 +8380,7 @@
         <v>217</v>
       </c>
       <c r="B4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -8429,7 +8436,7 @@
         <v>163</v>
       </c>
       <c r="B11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -8437,7 +8444,7 @@
         <v>162</v>
       </c>
       <c r="B12" t="s">
-        <v>226</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -8445,7 +8452,7 @@
         <v>161</v>
       </c>
       <c r="B13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -8453,7 +8460,7 @@
         <v>154</v>
       </c>
       <c r="B14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -8461,7 +8468,7 @@
         <v>153</v>
       </c>
       <c r="B15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -8469,23 +8476,23 @@
         <v>152</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -8493,7 +8500,7 @@
         <v>206</v>
       </c>
       <c r="B19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sorted annoying auto-correct date issue!
</commit_message>
<xml_diff>
--- a/Data/Trait_data_and_sources.xlsx
+++ b/Data/Trait_data_and_sources.xlsx
@@ -622,9 +622,6 @@
     <t>Distribution status - Source</t>
   </si>
   <si>
-    <t>Breeding habit (lentic/lotic)</t>
-  </si>
-  <si>
     <t>Larval body length - Min (mm)</t>
   </si>
   <si>
@@ -697,9 +694,6 @@
     <t>Species classified using the Red List criteria</t>
   </si>
   <si>
-    <t>Breeding habit</t>
-  </si>
-  <si>
     <t>Habitat data</t>
   </si>
   <si>
@@ -715,12 +709,6 @@
     <t>Range between the minimum and maximum numbers of years taken to complete the larval stage in the UK, where this is not a single value</t>
   </si>
   <si>
-    <t xml:space="preserve">Breeding habit - Source </t>
-  </si>
-  <si>
-    <t>Species are classified into two groups based on their preferred breeding habit, either lentic or lotic.</t>
-  </si>
-  <si>
     <t>A series of habitat types, species are given a 1 if they utilise the habitat in question.</t>
   </si>
   <si>
@@ -776,6 +764,18 @@
   </si>
   <si>
     <t>A variable describing a species emergence strategy: 1) Spring emergence = highly synchronised, 2) Summer emergence = temporally dispersed  emergence, 3) Type 3 Summer = Obligatorily univoltine species.</t>
+  </si>
+  <si>
+    <t>Breeding habitat (lentic/lotic)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Breeding habitat - Source </t>
+  </si>
+  <si>
+    <t>Breeding habitat</t>
+  </si>
+  <si>
+    <t>Species are classified into two groups based on their preferred breeding habitat, either lentic or lotic.</t>
   </si>
 </sst>
 </file>
@@ -1198,8 +1198,8 @@
   <dimension ref="A1:BP44"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V5" sqref="V5"/>
+      <pane xSplit="1" topLeftCell="AG1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AM11" sqref="AM11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1284,7 +1284,7 @@
         <v>190</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>149</v>
@@ -1296,7 +1296,7 @@
         <v>172</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Q1" s="3" t="s">
         <v>164</v>
@@ -1305,10 +1305,10 @@
         <v>179</v>
       </c>
       <c r="S1" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>203</v>
       </c>
       <c r="U1" s="3" t="s">
         <v>173</v>
@@ -1362,10 +1362,10 @@
         <v>195</v>
       </c>
       <c r="AL1" s="3" t="s">
-        <v>199</v>
+        <v>247</v>
       </c>
       <c r="AM1" s="3" t="s">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="AN1" s="5" t="s">
         <v>160</v>
@@ -1386,7 +1386,7 @@
         <v>155</v>
       </c>
       <c r="AT1" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AU1" s="6" t="s">
         <v>187</v>
@@ -1394,10 +1394,10 @@
     </row>
     <row r="2" spans="1:67">
       <c r="A2" s="3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>13</v>
@@ -1467,7 +1467,7 @@
         <v>1</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="Z2" s="3">
         <v>5</v>
@@ -1597,7 +1597,7 @@
         <v>178</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>9</v>
@@ -4001,10 +4001,10 @@
     </row>
     <row r="19" spans="1:67">
       <c r="A19" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>46</v>
@@ -4778,10 +4778,10 @@
     </row>
     <row r="24" spans="1:67">
       <c r="A24" s="3" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>46</v>
@@ -5395,10 +5395,10 @@
     </row>
     <row r="28" spans="1:67">
       <c r="A28" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>46</v>
@@ -5450,10 +5450,10 @@
         <v>1</v>
       </c>
       <c r="S28" s="3" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="T28" s="3" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="U28" s="3">
         <v>4</v>
@@ -5857,10 +5857,10 @@
     </row>
     <row r="31" spans="1:67">
       <c r="A31" s="13" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>46</v>
@@ -7947,10 +7947,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>208</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -7958,7 +7958,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -7966,7 +7966,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -8046,7 +8046,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -8054,7 +8054,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -8066,8 +8066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8078,34 +8078,34 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B3" t="s">
         <v>213</v>
-      </c>
-      <c r="B3" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B4" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -8113,7 +8113,7 @@
         <v>172</v>
       </c>
       <c r="B5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -8121,15 +8121,15 @@
         <v>164</v>
       </c>
       <c r="B6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
+        <v>218</v>
+      </c>
+      <c r="B7" t="s">
         <v>219</v>
-      </c>
-      <c r="B7" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -8137,7 +8137,7 @@
         <v>174</v>
       </c>
       <c r="B8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -8145,7 +8145,7 @@
         <v>197</v>
       </c>
       <c r="B9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -8153,7 +8153,7 @@
         <v>163</v>
       </c>
       <c r="B10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -8161,7 +8161,7 @@
         <v>162</v>
       </c>
       <c r="B11" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -8169,7 +8169,7 @@
         <v>161</v>
       </c>
       <c r="B12" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -8177,7 +8177,7 @@
         <v>154</v>
       </c>
       <c r="B13" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -8185,7 +8185,7 @@
         <v>153</v>
       </c>
       <c r="B14" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -8193,31 +8193,31 @@
         <v>152</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>224</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>231</v>
+        <v>249</v>
+      </c>
+      <c r="B16" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B18" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sorting the citations in the trait data and sources excel file
</commit_message>
<xml_diff>
--- a/Data/Trait_data_and_sources.xlsx
+++ b/Data/Trait_data_and_sources.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="20955" windowHeight="9465" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="20955" windowHeight="9465" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$V$39</definedName>
     <definedName name="Sex">[1]Lookups!$A$53:$A$56</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -553,30 +553,18 @@
     <t>Body size - Source</t>
   </si>
   <si>
-    <t>Corbet, S. &amp; Brooks, S. (2008) Dragonflies</t>
-  </si>
-  <si>
-    <t>Powell, D. (1999) A guide to the dragonflies of Great Britain.  Arlequin Press, Essex.</t>
-  </si>
-  <si>
     <t>EL</t>
   </si>
   <si>
     <t>Overwintering stage - Source</t>
   </si>
   <si>
-    <t>Smallshire, D. and Swash, A. 2010 Britain's Dragonflies: A field guide to the damselflies and dragonflies of Britain and Ireland WILDGuides, Old Basing, Hampshire, UK</t>
-  </si>
-  <si>
     <t>Flight period - Source</t>
   </si>
   <si>
     <t>Migratory - Source</t>
   </si>
   <si>
-    <t>Hammond, C. O. (1983) The dragonflies of Great Britain and Ireland.  Harley Books, Essex.</t>
-  </si>
-  <si>
     <t>Red list - Source</t>
   </si>
   <si>
@@ -592,30 +580,18 @@
     <t>Oviposition - Source</t>
   </si>
   <si>
-    <t>Daguet, C.A., French, G.C. and Taylor, P. (2008). The Odonata Red Data List for Great Britain. Species Status 11; 1-34. Joint Nature Conservation Committee, Peterborough</t>
-  </si>
-  <si>
     <t>Body length - Source</t>
   </si>
   <si>
     <t>Larval body length - Source</t>
   </si>
   <si>
-    <t>Dijkstra, K-D.B. and Lewington, R. 2006 Field Guide to the Dragonflies of Britain and Europe British Wildlife Publishing, Gillingham, Dorset, UK</t>
-  </si>
-  <si>
     <t>Shirt, D.P. (ed.) 1987 British Red Data Books 2: Insects Nature Conservancy Council</t>
   </si>
   <si>
-    <t>Cham, S. 2009 Field Guide to the larvae and exuviae of British Dragonflies Volume 2: Zygoptera British Dragonfly Society, Peterborough, UK</t>
-  </si>
-  <si>
     <t>Life cycle - Source</t>
   </si>
   <si>
-    <t>Cham, S. 2007 Field Guide to the larvae and exuviae of British Dragonflies Volume 1: Anisoptera British Dragonfly Society, Peterborough, UK</t>
-  </si>
-  <si>
     <t>Distribution status</t>
   </si>
   <si>
@@ -637,9 +613,6 @@
     <t>Habitat breadth</t>
   </si>
   <si>
-    <t xml:space="preserve">Brooks, S. &amp; Lewington, R. (2007) Field Guide to the Dragonflies and Damselflies of Great Britain and Ireland. Revised Edition. British Wildlife Publishing. Dorset, UK. </t>
-  </si>
-  <si>
     <t>d'Aguilar, J., Dommanget, J. L. &amp; Préchac, R. (1986) A field guide to the dragonflies of Britain, Europe and North Africa.  Collins. London, UK</t>
   </si>
   <si>
@@ -754,12 +727,6 @@
     <t>Vagrant</t>
   </si>
   <si>
-    <t>Merritt, R., Moore, N. W. &amp; Eversham, B. C. (1996) Atlas of the dragonflies of Britain and Ireland. HMSO Great Britain.</t>
-  </si>
-  <si>
-    <t>Brooks, S. (2013) Pers. Comm.</t>
-  </si>
-  <si>
     <t>A variable describing a species emergence strategy: 1) Spring emergence = highly synchronised, 2) Summer emergence = temporally dispersed  emergence, 3) Type 3 Summer = Obligatorily univoltine species.</t>
   </si>
   <si>
@@ -776,6 +743,39 @@
   </si>
   <si>
     <t>Species classified using the national Red List criteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brooks, S.J. &amp; Lewington, R. (2007) Field Guide to the Dragonflies and Damselflies of Great Britain and Ireland. Revised Edition. British Wildlife Publishing. Dorset, UK. </t>
+  </si>
+  <si>
+    <t>Brooks, S.J. (2013) Pers. Comm.</t>
+  </si>
+  <si>
+    <t>Corbet, P.S. &amp; Brooks, S.J. (2008) Dragonflies. Collins, London, UK</t>
+  </si>
+  <si>
+    <t>Hammond, C.O. (1983) The dragonflies of Great Britain and Ireland.  Harley Books, Essex. UK</t>
+  </si>
+  <si>
+    <t>Powell, D. (1999) A guide to the dragonflies of Great Britain.  Arlequin Press, Essex. UK</t>
+  </si>
+  <si>
+    <t>Daguet, C.A., French, G.C. and Taylor, P. (2008). The Odonata Red Data List for Great Britain. Species Status 11; 1-34. Joint Nature Conservation Committee, Peterborough, UK</t>
+  </si>
+  <si>
+    <t>Smallshire, D. and Swash, A. (2010) Britain's Dragonflies: A field guide to the damselflies and dragonflies of Britain and Ireland WILDGuides, Old Basing, Hampshire, UK</t>
+  </si>
+  <si>
+    <t>Dijkstra, K-D.B. and Lewington, R. (2006) Field Guide to the Dragonflies of Britain and Europe British Wildlife Publishing, Gillingham, Dorset, UK</t>
+  </si>
+  <si>
+    <t>Cham, S. (2009) Field Guide to the larvae and exuviae of British Dragonflies Volume 2: Zygoptera British Dragonfly Society, Peterborough, UK</t>
+  </si>
+  <si>
+    <t>Cham, S. (2007) Field Guide to the larvae and exuviae of British Dragonflies Volume 1: Anisoptera British Dragonfly Society, Peterborough, UK</t>
+  </si>
+  <si>
+    <t>Merritt, R., Moore, N.W. &amp; Eversham, B.C. (1996) Atlas of the dragonflies of Britain and Ireland. HMSO Great Britain.</t>
   </si>
 </sst>
 </file>
@@ -1272,76 +1272,76 @@
         <v>150</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>149</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>172</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="Q1" s="3" t="s">
         <v>164</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="U1" s="3" t="s">
         <v>173</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="W1" s="3" t="s">
         <v>174</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="AA1" s="3" t="s">
         <v>163</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="AC1" s="3" t="s">
         <v>162</v>
       </c>
       <c r="AD1" s="3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="AE1" s="3" t="s">
         <v>161</v>
       </c>
       <c r="AF1" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="AG1" s="3" t="s">
         <v>154</v>
       </c>
       <c r="AH1" s="6" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="AI1" s="3" t="s">
         <v>153</v>
@@ -1350,13 +1350,13 @@
         <v>152</v>
       </c>
       <c r="AK1" s="3" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="AL1" s="3" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="AM1" s="3" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="AN1" s="5" t="s">
         <v>160</v>
@@ -1377,18 +1377,18 @@
         <v>155</v>
       </c>
       <c r="AT1" s="3" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="AU1" s="6" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:67">
       <c r="A2" s="3" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>13</v>
@@ -1458,7 +1458,7 @@
         <v>1</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="Z2" s="3">
         <v>1</v>
@@ -1586,10 +1586,10 @@
         <v>1</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>9</v>
@@ -1738,7 +1738,7 @@
         <v>1</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="R4" s="3">
         <v>1</v>
@@ -1893,7 +1893,7 @@
         <v>1</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="R5" s="3">
         <v>1</v>
@@ -2054,7 +2054,7 @@
         <v>1</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="R6" s="3">
         <v>3</v>
@@ -3993,10 +3993,10 @@
     </row>
     <row r="19" spans="1:67">
       <c r="A19" s="3" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>46</v>
@@ -4769,10 +4769,10 @@
     </row>
     <row r="24" spans="1:67">
       <c r="A24" s="3" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>46</v>
@@ -5384,10 +5384,10 @@
     </row>
     <row r="28" spans="1:67">
       <c r="A28" s="3" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>46</v>
@@ -5439,10 +5439,10 @@
         <v>1</v>
       </c>
       <c r="S28" s="3" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="T28" s="3" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="U28" s="3">
         <v>4</v>
@@ -5850,10 +5850,10 @@
     </row>
     <row r="31" spans="1:67">
       <c r="A31" s="13" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>46</v>
@@ -7805,7 +7805,7 @@
         <v>1</v>
       </c>
       <c r="Q44" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="R44" s="3">
         <v>6</v>
@@ -7933,8 +7933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7944,10 +7944,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -7955,7 +7955,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>204</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -7963,7 +7963,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -7971,7 +7971,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>176</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -7979,7 +7979,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>183</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -7987,7 +7987,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>177</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -7995,7 +7995,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>180</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -8003,7 +8003,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>189</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -8011,7 +8011,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>192</v>
+        <v>247</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -8019,7 +8019,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -8027,7 +8027,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>194</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -8035,7 +8035,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>196</v>
+        <v>249</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -8043,7 +8043,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -8051,7 +8051,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -8063,7 +8063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -8075,34 +8075,34 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="B1" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="B2" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B3" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="B4" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -8110,7 +8110,7 @@
         <v>172</v>
       </c>
       <c r="B5" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -8118,15 +8118,15 @@
         <v>164</v>
       </c>
       <c r="B6" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="B7" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -8134,15 +8134,15 @@
         <v>174</v>
       </c>
       <c r="B8" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B9" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -8150,7 +8150,7 @@
         <v>163</v>
       </c>
       <c r="B10" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -8158,7 +8158,7 @@
         <v>162</v>
       </c>
       <c r="B11" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -8166,7 +8166,7 @@
         <v>161</v>
       </c>
       <c r="B12" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -8174,7 +8174,7 @@
         <v>154</v>
       </c>
       <c r="B13" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -8182,7 +8182,7 @@
         <v>153</v>
       </c>
       <c r="B14" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -8190,31 +8190,31 @@
         <v>152</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="B16" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="B17" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B18" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>